<commit_message>
ECP-962: adds property frequency on turnover
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>OXF-001</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>GBP</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>MONTHLY</t>
+  </si>
+  <si>
+    <t>QUARTERLY</t>
   </si>
 </sst>
 </file>
@@ -120,7 +129,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -142,6 +151,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -189,7 +200,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="64">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -231,6 +242,7 @@
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
@@ -251,6 +263,7 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -588,9 +601,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
@@ -606,7 +621,7 @@
     <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -620,25 +635,28 @@
         <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -651,20 +669,23 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2">
         <v>14814.671999999999</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>12345.56</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>123</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -677,16 +698,20 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2">
         <v>2345.67</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2"/>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ECP-962: creates own frequency for turnover
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
@@ -78,7 +78,7 @@
     <t>MONTHLY</t>
   </si>
   <si>
-    <t>QUARTERLY</t>
+    <t>DAILY</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -618,7 +618,7 @@
     <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">

</xml_diff>

<commit_message>
ECP-962: some renaming and first sketch import manager
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
@@ -33,12 +33,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>turnover gross amount</t>
-  </si>
-  <si>
-    <t>turnover net amount</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -48,9 +42,6 @@
     <t>non comparable flag</t>
   </si>
   <si>
-    <t>turnover purchase count</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -79,6 +70,15 @@
   </si>
   <si>
     <t>DAILY</t>
+  </si>
+  <si>
+    <t>gross amount</t>
+  </si>
+  <si>
+    <t>net amount</t>
+  </si>
+  <si>
+    <t>purchase count</t>
   </si>
 </sst>
 </file>
@@ -603,9 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
@@ -632,33 +630,33 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -667,10 +665,10 @@
         <v>43466</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2">
         <v>14814.671999999999</v>
@@ -682,12 +680,12 @@
         <v>123</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -696,10 +694,10 @@
         <v>43556</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2">
         <v>2345.67</v>
@@ -709,10 +707,10 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ECP-962: enhances turnover import to work with jdbc fixture
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="5920" windowWidth="31080" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="9560" yWindow="5920" windowWidth="36040" windowHeight="17000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TurnoverImport" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>OXF-001</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>purchase count</t>
+  </si>
+  <si>
+    <t>occupancyStartDate</t>
+  </si>
+  <si>
+    <t>reportedAt</t>
+  </si>
+  <si>
+    <t>reportedBy</t>
+  </si>
+  <si>
+    <t>manager abc</t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -194,13 +206,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="78">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -243,6 +270,13 @@
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
@@ -264,6 +298,13 @@
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,25 +642,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="47.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.1640625" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -627,34 +674,43 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -662,28 +718,37 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D2" s="1">
         <v>43466</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>14814.671999999999</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>12345.56</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>123</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="3">
+        <v>43423.462736111112</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -691,26 +756,35 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
+        <v>40374</v>
+      </c>
+      <c r="D3" s="1">
         <v>43556</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>2345.67</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3">
+      <c r="H3" s="2"/>
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>13</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="3">
+        <v>43423.462736111112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ECP-962: updates turnover import
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9560" yWindow="5920" windowWidth="36040" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28080" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TurnoverImport" sheetId="5" r:id="rId1"/>
@@ -19,32 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>OXF-001</t>
   </si>
   <si>
-    <t>lease reference</t>
-  </si>
-  <si>
-    <t>unit reference</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>currency reference</t>
-  </si>
-  <si>
-    <t>non comparable flag</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
     <t>This is non comparable because of some reason</t>
   </si>
   <si>
@@ -63,34 +42,67 @@
     <t>GBP</t>
   </si>
   <si>
-    <t>frequency</t>
-  </si>
-  <si>
     <t>MONTHLY</t>
   </si>
   <si>
     <t>DAILY</t>
   </si>
   <si>
-    <t>gross amount</t>
-  </si>
-  <si>
-    <t>net amount</t>
-  </si>
-  <si>
-    <t>purchase count</t>
-  </si>
-  <si>
-    <t>occupancyStartDate</t>
-  </si>
-  <si>
-    <t>reportedAt</t>
-  </si>
-  <si>
-    <t>reportedBy</t>
-  </si>
-  <si>
     <t>manager abc</t>
+  </si>
+  <si>
+    <t>Gross Amount Previous Year</t>
+  </si>
+  <si>
+    <t>Net Amount Previous Year</t>
+  </si>
+  <si>
+    <t>Purchase Count Previous Year</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Unit Reference</t>
+  </si>
+  <si>
+    <t>Lease Reference</t>
+  </si>
+  <si>
+    <t>Lease Name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Gross Amount</t>
+  </si>
+  <si>
+    <t>Net Amount</t>
+  </si>
+  <si>
+    <t>Purchase Count</t>
+  </si>
+  <si>
+    <t>Non Comparable Flag</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Occupancy Start Date</t>
+  </si>
+  <si>
+    <t>Reported At</t>
+  </si>
+  <si>
+    <t>Reported By</t>
   </si>
 </sst>
 </file>
@@ -100,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -123,6 +135,12 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,7 +159,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="78">
+  <cellStyleXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -220,14 +238,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="78">
+  <cellStyles count="114">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -277,6 +332,24 @@
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
@@ -305,6 +378,24 @@
     <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -642,77 +733,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.1640625" customWidth="1"/>
-    <col min="12" max="12" width="18.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="23.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:18" ht="14">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -724,10 +829,10 @@
         <v>43466</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G2" s="2">
         <v>14814.671999999999</v>
@@ -739,18 +844,18 @@
         <v>123</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="N2" s="3">
         <v>43423.462736111112</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -762,10 +867,10 @@
         <v>43556</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G3" s="2">
         <v>2345.67</v>
@@ -775,17 +880,20 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="N3" s="3">
         <v>43423.462736111112</v>
       </c>
+    </row>
+    <row r="6" spans="1:18" ht="14">
+      <c r="C6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
ECP-1033: now calculates net from gross (instead of gross from net) for Swe
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/turnover/fixtures/TurnoverImport.xlsx
@@ -735,7 +735,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
@@ -875,7 +877,9 @@
       <c r="G3" s="2">
         <v>2345.67</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
       <c r="I3">
         <v>1</v>
       </c>

</xml_diff>